<commit_message>
SonarQube fixes and Excell update
</commit_message>
<xml_diff>
--- a/Docs/L_01/Lab01_ReviewReport 2.xlsx
+++ b/Docs/L_01/Lab01_ReviewReport 2.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28706"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{325487CD-C5B8-4570-A977-097EB7BBFBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11505" tabRatio="650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11505" tabRatio="650" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="107">
   <si>
     <t>do not print this form</t>
   </si>
@@ -313,19 +312,68 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
+  </si>
+  <si>
+    <t>String literals should not be duplicated</t>
+  </si>
+  <si>
+    <t>Payment allert</t>
+  </si>
+  <si>
+    <t>System.out.println("--------------------------");</t>
+  </si>
+  <si>
+    <t>System.out.println(line);</t>
+  </si>
+  <si>
+    <t>Empty arrays and collections should be returned instead of null</t>
+  </si>
+  <si>
+    <t>Payment Service</t>
+  </si>
+  <si>
+    <t>return null;</t>
+  </si>
+  <si>
+    <t>return Collections.emptyList();</t>
+  </si>
+  <si>
+    <t>Resources should be closed</t>
+  </si>
+  <si>
+    <t>Payment Repository</t>
+  </si>
+  <si>
+    <t>try(BufferedReader br = new BufferedReader(new FileReader(file))) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try(BufferedWriter bw = new BufferedWriter(new FileWriter(file))) </t>
+  </si>
+  <si>
+    <t>Methods should not be empty</t>
+  </si>
+  <si>
+    <t>MenuRepository</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -490,84 +538,85 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,9 +635,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -626,7 +675,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -698,7 +747,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -871,7 +920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -881,7 +930,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -894,134 +943,134 @@
     <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="24" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="20"/>
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="16" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="16" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="16" t="s">
+      <c r="E5" s="27"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>45722</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="20"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
@@ -1034,15 +1083,15 @@
       <c r="E9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="20"/>
-      <c r="B10" s="16">
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="15">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1054,15 +1103,15 @@
       <c r="E10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="20"/>
-      <c r="B11" s="16">
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="15">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -1075,15 +1124,15 @@
       <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="20"/>
-      <c r="B12" s="16">
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="15">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -1096,15 +1145,15 @@
       <c r="E12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="20"/>
-      <c r="B13" s="16">
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1115,15 +1164,15 @@
       <c r="E13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="20"/>
-      <c r="B14" s="16">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1134,44 +1183,44 @@
       <c r="E14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="20"/>
-      <c r="B15" s="16">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="20"/>
-      <c r="B16" s="16">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="16">
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1179,85 +1228,85 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="16">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="16">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="21"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="16">
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="21"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="16">
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="21"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="16">
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="21"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="16">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="21"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="16">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="21"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="16">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="21"/>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="20"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="19"/>
       <c r="C27" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="11"/>
-      <c r="E27" s="17">
+      <c r="E27" s="16">
         <v>1.1875</v>
       </c>
     </row>
@@ -1276,17 +1325,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -1297,134 +1346,136 @@
     <col min="10" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="24" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="20"/>
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="16" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="16" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="16" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+      <c r="D6" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>45722</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="20"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
@@ -1437,15 +1488,15 @@
       <c r="E9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="20"/>
-      <c r="B10" s="16">
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="15">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1455,15 +1506,15 @@
       <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="20"/>
-      <c r="B11" s="16">
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="15">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -1474,15 +1525,15 @@
       <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="20"/>
-      <c r="B12" s="16">
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="15">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -1493,15 +1544,15 @@
       <c r="E12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="20"/>
-      <c r="B13" s="16">
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1512,15 +1563,15 @@
       <c r="E13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" ht="30.75">
-      <c r="A14" s="20"/>
-      <c r="B14" s="16">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1531,48 +1582,48 @@
       <c r="E14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="30.75">
-      <c r="A15" s="20"/>
-      <c r="B15" s="16">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="20"/>
-      <c r="B16" s="16">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="16">
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1580,8 +1631,8 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="16">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1589,8 +1640,8 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="16">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1598,8 +1649,8 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="16">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1607,8 +1658,8 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="16">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1616,8 +1667,8 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="16">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -1625,8 +1676,8 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="16">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1634,8 +1685,8 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="16">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1643,8 +1694,8 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="16">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -1652,8 +1703,8 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="16">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="15">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -1661,13 +1712,13 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="20"/>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="19"/>
       <c r="C28" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="11"/>
-      <c r="E28" s="17">
+      <c r="E28" s="16">
         <v>1.0625</v>
       </c>
     </row>
@@ -1686,17 +1737,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -1708,134 +1759,136 @@
     <col min="10" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="24" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="20"/>
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="16" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="15">
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="16" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="16" t="s">
+      <c r="E5" s="33"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="15">
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+      <c r="D6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="20"/>
+      <c r="D7" s="21">
+        <v>45731</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
@@ -1848,15 +1901,15 @@
       <c r="E9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" ht="30.75">
-      <c r="A10" s="20"/>
-      <c r="B10" s="16">
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="15">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1868,15 +1921,15 @@
       <c r="E10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" ht="30.75">
-      <c r="A11" s="20"/>
-      <c r="B11" s="16">
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="15">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -1889,15 +1942,15 @@
       <c r="E11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10" ht="30.75">
-      <c r="A12" s="20"/>
-      <c r="B12" s="16">
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="15">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
@@ -1910,15 +1963,15 @@
       <c r="E12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10" ht="30.75">
-      <c r="A13" s="20"/>
-      <c r="B13" s="16">
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1931,15 +1984,15 @@
       <c r="E13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" ht="30.75">
-      <c r="A14" s="20"/>
-      <c r="B14" s="16">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -1952,15 +2005,15 @@
       <c r="E14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="30.75">
-      <c r="A15" s="20"/>
-      <c r="B15" s="16">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1973,15 +2026,15 @@
       <c r="E15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" ht="30.75">
-      <c r="A16" s="20"/>
-      <c r="B16" s="16">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1992,14 +2045,14 @@
       <c r="E16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="16">
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2011,8 +2064,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="16">
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2026,8 +2079,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="16">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2041,8 +2094,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="30.75">
-      <c r="B20" s="16">
+    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2056,8 +2109,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="16">
+    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2071,8 +2124,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="30.75">
-      <c r="B22" s="16">
+    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2086,8 +2139,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="16">
+    <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2101,8 +2154,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="30.75">
-      <c r="B24" s="16">
+    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2116,8 +2169,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="16">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -2125,8 +2178,8 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="16">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="15">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -2134,8 +2187,8 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="16">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="15">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -2143,8 +2196,8 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="16">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="15">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -2152,8 +2205,8 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="16">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="15">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -2161,8 +2214,8 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="16">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="15">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -2170,13 +2223,15 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="20"/>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="19"/>
       <c r="C32" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D32" s="11"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="16">
+        <v>1.1875</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2193,17 +2248,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
@@ -2216,102 +2271,118 @@
     <col min="10" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="24" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="20"/>
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="16" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+      <c r="I3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="15">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="16" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="I4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="15">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="16" t="s">
+      <c r="D5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="20"/>
+      <c r="I5" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="15">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="20"/>
+      <c r="D6" s="21">
+        <v>45731</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
@@ -2327,103 +2398,138 @@
       <c r="F9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="20"/>
-      <c r="B10" s="16">
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="15">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="20"/>
-      <c r="B11" s="16">
+      <c r="C10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="15">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="20"/>
-      <c r="B12" s="16">
+      <c r="C11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="15">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="20"/>
-      <c r="B13" s="16">
+      <c r="F12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="20"/>
-      <c r="B14" s="16">
+      <c r="F13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="20"/>
-      <c r="B15" s="16">
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="20"/>
-      <c r="B16" s="16">
+      <c r="F15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -2431,13 +2537,13 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="16">
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2446,8 +2552,8 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="16">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2456,8 +2562,8 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="16">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2466,8 +2572,8 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="16">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2476,8 +2582,8 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="16">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2486,8 +2592,8 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="16">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2496,8 +2602,8 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="16">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2506,8 +2612,8 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="16">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2516,8 +2622,8 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="16">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -2526,8 +2632,8 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="16">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="15">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -2536,8 +2642,8 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="16">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="15">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -2546,8 +2652,8 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="16">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="15">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -2556,8 +2662,8 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="16">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="15">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -2566,8 +2672,8 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6">
-      <c r="B30" s="16">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="15">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -2576,17 +2682,19 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6">
-      <c r="B32" s="20"/>
-      <c r="C32" s="35" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="19"/>
+      <c r="C32" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="15"/>
-    </row>
-    <row r="35" spans="6:6">
-      <c r="F35" s="20"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="37">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>